<commit_message>
Ažuriranje i nova dokumentacija
Ažurirana i nova dokumentacija
</commit_message>
<xml_diff>
--- a/Projekt/PB_0 Popis dolumentacije za projekt e-Inspektor, Tim -T27_Plan B.xlsx
+++ b/Projekt/PB_0 Popis dolumentacije za projekt e-Inspektor, Tim -T27_Plan B.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
   <si>
     <t>Rbr.</t>
   </si>
@@ -249,6 +249,75 @@
   </si>
   <si>
     <t>izmjene plana</t>
+  </si>
+  <si>
+    <t>14.</t>
+  </si>
+  <si>
+    <t>PB_14</t>
+  </si>
+  <si>
+    <t>24.04.2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifikacija slučajeva korištenja VIES registra </t>
+  </si>
+  <si>
+    <t>15.</t>
+  </si>
+  <si>
+    <t>PB_15</t>
+  </si>
+  <si>
+    <t>Analiza poslovnih procesa vezanih uz PDV registar</t>
+  </si>
+  <si>
+    <t>25.04.2014.</t>
+  </si>
+  <si>
+    <t>Analiza funkcionalnosti PDV registra</t>
+  </si>
+  <si>
+    <t>Specifikacija UC020 Upravljanje sadržajima VIES registra</t>
+  </si>
+  <si>
+    <t>16.</t>
+  </si>
+  <si>
+    <t>PB_16</t>
+  </si>
+  <si>
+    <t>Specifikacija UC300 Unos PDV podataka u registar</t>
+  </si>
+  <si>
+    <t>17.</t>
+  </si>
+  <si>
+    <t>PB_17</t>
+  </si>
+  <si>
+    <t>18.</t>
+  </si>
+  <si>
+    <t>PB_18</t>
+  </si>
+  <si>
+    <t>Specifikacija UC301 Pretraživanje PDV podataka</t>
+  </si>
+  <si>
+    <t>Specifikacija UC302 Ažuriranje registra PDV podataka</t>
+  </si>
+  <si>
+    <t>19.</t>
+  </si>
+  <si>
+    <t>PB_19</t>
+  </si>
+  <si>
+    <t>Specifikacija UC303 Kontrola PDV podataka</t>
+  </si>
+  <si>
+    <t>Specifikacija slučajeva korištenja</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1472,53 +1541,125 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="14"/>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>

</xml_diff>

<commit_message>
UC030 Upravljanje funkcionalnostima PDV registra
UC030, SD030, AD030 i prateća dokumentacija za upravljanje
funkcionalnostima PDV registra
</commit_message>
<xml_diff>
--- a/Projekt/PB_0 Popis dolumentacije za projekt e-Inspektor, Tim -T27_Plan B.xlsx
+++ b/Projekt/PB_0 Popis dolumentacije za projekt e-Inspektor, Tim -T27_Plan B.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>Rbr.</t>
   </si>
@@ -341,9 +341,6 @@
     <t>PB_21</t>
   </si>
   <si>
-    <t>Specifikacija slučajeva korištenja UC102 Upravljanjem funkcionalnostima aplikacije</t>
-  </si>
-  <si>
     <t>05.05.2014.</t>
   </si>
   <si>
@@ -357,6 +354,21 @@
   </si>
   <si>
     <t>Popis ekrana aplikacije</t>
+  </si>
+  <si>
+    <t>23.</t>
+  </si>
+  <si>
+    <t>PB_23</t>
+  </si>
+  <si>
+    <t>08.05.2014.</t>
+  </si>
+  <si>
+    <t>Specifikacija UC030 Upravljanje funkcionalnostima PDV registra</t>
+  </si>
+  <si>
+    <t>Specifikacija UC102 Upravljanjem funkcionalnostima aplikacije</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1243,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1728,13 +1740,13 @@
         <v>106</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>99</v>
@@ -1742,31 +1754,43 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="D27" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F27" s="14" t="s">
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="14"/>
+      <c r="B28" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>

</xml_diff>